<commit_message>
Updates to tagging prompts.
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dvagov-my.sharepoint.com/personal/ryan_powers3_va_gov/Documents/Documents/Medallia Text Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{79DC7C6D-0777-4471-A368-A05D08D24BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{560A2BD4-7EFA-4199-BF7E-9734AF417170}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{79DC7C6D-0777-4471-A368-A05D08D24BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FF19F5-AB96-44E4-A7F7-2F93428349E9}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="25185" windowHeight="13800" xr2:uid="{7599146C-7E46-468A-91C1-B54BA2166AD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7599146C-7E46-468A-91C1-B54BA2166AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Prompt</t>
   </si>
@@ -50,20 +50,44 @@
     <t>Sentiment</t>
   </si>
   <si>
-    <t>Classify the topic of the following comment:
+    <t>Instructions:
+    - Choose one of the following: Positive, Negative.
+    - Choose the sentiment of the user feedback comment based on the tone and context of the comment.</t>
+  </si>
+  <si>
+    <t>You are an expert in classifying user feedback into specific categories (tags). Each tag corresponds to a specific theme of user feedback. Below are the predefined tags and their meanings:
+- **Ease of use**: The comment mentions how intuitive, simple, or complicated the site or service is.
+- **Findability/Nav**: The comment mentions difficulty in finding information, navigating the site, or understanding its structure.
+- **Integration**: The comment discusses changes, compatibility, or integration with other systems.
+- **Early pop up**: The comment mentions issues with prompts or pop-ups that appear at an inappropriate time.
+- **Other**: The comment mentions positive feedback or does not fit the other tags.
+Here are some examples of correctly tagged comments:
+1. Comment: "This site is very confusing! We are not tech-savvy."
+   Tag: Ease of use
+2. Comment: "I couldn’t find the prescription refill section easily."
+   Tag: Findability/Nav
+3. Comment: "The dropdown menus are overly complex and unintuitive."
+   Tag: Findability/Nav
+4. Comment: "The new design keeps changing and feels unfamiliar."
+   Tag: Integration
+5. Comment: "I appreciate the messaging system. It works great!"
+   Tag: Other
+Now, read the following comment carefully and assign the most appropriate tag. Select only one tag that best describes the feedback.
+Comment: "{comment}"
+Output format:
+Tag: &lt;Selected Tag&gt;</t>
+  </si>
+  <si>
+    <t>Act as a customer feedback analysis expert tasked with tagging user comments. Use the provided examples and tags to identify the theme of the comment. Classify the topic of the following comment:
 Comment: "{comment}"
 Choose a tag from the following list:
 Tags: {TAGS}
 Instructions:
-- Select one tag from the list above that best describes the main point of the comment.
-- If no tag fits, return "Other".
+1. Carefully read the comment.
+2. Match it to the tag that best captures the user's primary concern or feedback.
+3. If uncertain, choose the most closely related tag.
 Output format:
 Tag: [Selected Tag]</t>
-  </si>
-  <si>
-    <t>Instructions:
-    - Choose one of the following: Positive, Negative.
-    - Choose the sentiment of the user feedback comment based on the tone and context of the comment.</t>
   </si>
 </sst>
 </file>
@@ -422,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A8F853-01E8-4EE8-A513-D244A95476AC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,12 +465,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -454,6 +478,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="264" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>